<commit_message>
Upated RTM, removed antiquated Req ID doc
</commit_message>
<xml_diff>
--- a/Requirements_Traceability_Matrix_FuzzyFarmer.xlsx
+++ b/Requirements_Traceability_Matrix_FuzzyFarmer.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SchoolProject\FuzzyFarmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2F4C31B-F886-4C80-97E6-AAF1CDAD4368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E85C8-3A7E-4CD5-9265-D05345B5FE20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42615" yWindow="3465" windowWidth="19200" windowHeight="10065" xr2:uid="{42DA7BC4-4D15-4FD9-ACCE-6D17A319C051}"/>
+    <workbookView xWindow="0" yWindow="2310" windowWidth="19200" windowHeight="10070" xr2:uid="{42DA7BC4-4D15-4FD9-ACCE-6D17A319C051}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Req Traceability Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirements and Test Scenarios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
   <si>
     <t xml:space="preserve">Requirements ID            </t>
   </si>
@@ -42,6 +43,162 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Field Themed Background</t>
+  </si>
+  <si>
+    <t>Boulders/Asthetics applied as suitable for level</t>
+  </si>
+  <si>
+    <t>Collectable fuzzies</t>
+  </si>
+  <si>
+    <t>Top-Down, First-Person, or Third Person Interface</t>
+  </si>
+  <si>
+    <t>Mouse, Keyboard, or combination of controls (determined by dev)</t>
+  </si>
+  <si>
+    <t>Count Down Timer</t>
+  </si>
+  <si>
+    <t>Test Scenarios/Cases</t>
+  </si>
+  <si>
+    <t>Boulders and aesthetic items add to experience, not distract</t>
+  </si>
+  <si>
+    <t>Requirements ID:</t>
+  </si>
+  <si>
+    <t>ID: 1</t>
+  </si>
+  <si>
+    <t>ID: 2</t>
+  </si>
+  <si>
+    <t>ID: 3</t>
+  </si>
+  <si>
+    <t>ID: 4</t>
+  </si>
+  <si>
+    <t>ID: 5</t>
+  </si>
+  <si>
+    <t>ID: 6</t>
+  </si>
+  <si>
+    <t>ID: 7</t>
+  </si>
+  <si>
+    <t>ID: 8</t>
+  </si>
+  <si>
+    <t>ID: 9</t>
+  </si>
+  <si>
+    <t>TC: 1</t>
+  </si>
+  <si>
+    <t>TC: 2</t>
+  </si>
+  <si>
+    <t>TC: 3</t>
+  </si>
+  <si>
+    <t>TC: 4</t>
+  </si>
+  <si>
+    <t>TC: 5</t>
+  </si>
+  <si>
+    <t>TC: 6</t>
+  </si>
+  <si>
+    <t>TC: 7</t>
+  </si>
+  <si>
+    <t>TC: 8</t>
+  </si>
+  <si>
+    <t>ID: 10</t>
+  </si>
+  <si>
+    <t>SFX for finding/collecting</t>
+  </si>
+  <si>
+    <t>ID: 11</t>
+  </si>
+  <si>
+    <t>Suitable for casual gamers years 5+</t>
+  </si>
+  <si>
+    <t>ID: 12</t>
+  </si>
+  <si>
+    <t>Random fuzzy spawn location**</t>
+  </si>
+  <si>
+    <t>Ambient noise/music may be included as background audio**</t>
+  </si>
+  <si>
+    <t>ID: 12 **</t>
+  </si>
+  <si>
+    <t>ID: 5 **</t>
+  </si>
+  <si>
+    <t>ID: 3 **</t>
+  </si>
+  <si>
+    <t>Level enclosed by fence but otherwise free movement</t>
+  </si>
+  <si>
+    <t>Random Quest/Requirement with interface that informs user of fuzzy goal</t>
+  </si>
+  <si>
+    <t>ID: 13</t>
+  </si>
+  <si>
+    <t>Successful or Unsuccessful Rating</t>
+  </si>
+  <si>
+    <t>ID: 14</t>
+  </si>
+  <si>
+    <t>Successful rewards player with a Fuzzy</t>
+  </si>
+  <si>
+    <t>Explore playfield</t>
+  </si>
+  <si>
+    <t>Obtain quests/start timed round</t>
+  </si>
+  <si>
+    <t>Play through timer countdown</t>
+  </si>
+  <si>
+    <t>Try to collect pigs</t>
+  </si>
+  <si>
+    <t>Try to collect giraffes</t>
+  </si>
+  <si>
+    <t>Complete acquired quest</t>
+  </si>
+  <si>
+    <t>Verify collectible fuzzies are attainable given number of them on field</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ID: 15</t>
+  </si>
+  <si>
+    <t>Unsuccessful rating when timer expires</t>
   </si>
 </sst>
 </file>
@@ -57,15 +214,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -73,12 +236,141 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419BEFA8-3027-45F1-B8DB-451EA99CABB9}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -405,47 +697,565 @@
     <col min="2" max="2" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>3</v>
+      </c>
+      <c r="K2" s="4">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2</v>
+      </c>
+      <c r="M2" s="4">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>2</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A03CD8-9C7E-4A14-A460-0BFB8C17A0D1}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="F1">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="G1">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="H1">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="I1">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="J1">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="K1">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="L1">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted timer, updated RTM
</commit_message>
<xml_diff>
--- a/Requirements_Traceability_Matrix_FuzzyFarmer.xlsx
+++ b/Requirements_Traceability_Matrix_FuzzyFarmer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SchoolProject\FuzzyFarmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E85C8-3A7E-4CD5-9265-D05345B5FE20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B580B10-43C1-4116-ABE2-C1D23514B6DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2310" windowWidth="19200" windowHeight="10070" xr2:uid="{42DA7BC4-4D15-4FD9-ACCE-6D17A319C051}"/>
+    <workbookView xWindow="42165" yWindow="2775" windowWidth="19200" windowHeight="10065" activeTab="1" xr2:uid="{42DA7BC4-4D15-4FD9-ACCE-6D17A319C051}"/>
   </bookViews>
   <sheets>
     <sheet name="Req Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
   <si>
     <t xml:space="preserve">Requirements ID            </t>
   </si>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419BEFA8-3027-45F1-B8DB-451EA99CABB9}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,16 +780,16 @@
         <v>3</v>
       </c>
       <c r="K2" s="4">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4">
         <v>3</v>
       </c>
-      <c r="L2" s="4">
+      <c r="M2" s="4">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4">
         <v>2</v>
-      </c>
-      <c r="M2" s="4">
-        <v>4</v>
-      </c>
-      <c r="N2" s="4">
-        <v>1</v>
       </c>
       <c r="O2" s="4">
         <v>2</v>
@@ -872,7 +872,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -884,12 +884,8 @@
       <c r="J5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -959,7 +955,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -973,7 +969,9 @@
       <c r="L8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
         <v>52</v>
@@ -988,7 +986,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -999,7 +997,9 @@
         <v>52</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
         <v>52</v>
@@ -1007,11 +1007,15 @@
       <c r="K9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="M9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1021,7 +1025,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1030,13 +1034,19 @@
         <v>52</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="M10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1058,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A03CD8-9C7E-4A14-A460-0BFB8C17A0D1}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>